<commit_message>
Add order parser and tests.
</commit_message>
<xml_diff>
--- a/tests/fixtures/orders.xlsx
+++ b/tests/fixtures/orders.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Январь" sheetId="1" state="visible" r:id="rId2"/>
@@ -335,11 +335,11 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
   </cols>
@@ -498,15 +498,15 @@
         <v>44223</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="4" t="n">
-        <v>44224</v>
+      <c r="C15" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,7 +607,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -630,7 +630,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -653,7 +653,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -676,7 +676,7 @@
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.71"/>
   </cols>
@@ -953,7 +953,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.54"/>
   </cols>
@@ -991,7 +991,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="n">
@@ -1026,7 +1026,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.43"/>
   </cols>
@@ -1060,14 +1060,14 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1312,7 +1312,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1335,7 +1335,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1358,7 +1358,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>